<commit_message>
Dialog Trigger für Katze eingebaut
</commit_message>
<xml_diff>
--- a/CastingÜbersicht.xlsx
+++ b/CastingÜbersicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxpf\BachelorGame2024\BachelorGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE38586-5FF3-446F-A89E-414E0FA36184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BECA4A-D0FC-4FE7-B60C-83C0B500D29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="241">
   <si>
     <t>Katze</t>
   </si>
@@ -747,6 +747,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bisschen zu viel </t>
+  </si>
+  <si>
+    <t>Sophia Schröter</t>
   </si>
 </sst>
 </file>
@@ -2288,10 +2291,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF958A6-1110-4659-BA13-803572FE8662}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2596,153 +2599,156 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E26" t="s">
         <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>197</v>
+        <v>235</v>
       </c>
       <c r="E27" t="s">
         <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>198</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>199</v>
+        <v>238</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E28" t="s">
         <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>233</v>
+        <v>197</v>
       </c>
       <c r="E29" t="s">
         <v>9</v>
       </c>
       <c r="F29" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>104</v>
+        <v>199</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E30" t="s">
-        <v>87</v>
-      </c>
-      <c r="F30" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>207</v>
-      </c>
-      <c r="C31" t="s">
-        <v>75</v>
+        <v>233</v>
       </c>
       <c r="E31" t="s">
         <v>9</v>
+      </c>
+      <c r="F31" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>202</v>
+        <v>104</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E32" t="s">
-        <v>9</v>
+        <v>87</v>
+      </c>
+      <c r="F32" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>55</v>
+        <v>207</v>
+      </c>
+      <c r="C33" t="s">
+        <v>75</v>
       </c>
       <c r="E33" t="s">
         <v>9</v>
-      </c>
-      <c r="F33" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>203</v>
+        <v>202</v>
+      </c>
+      <c r="C34" t="s">
+        <v>72</v>
       </c>
       <c r="E34" t="s">
         <v>9</v>
-      </c>
-      <c r="F34" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>204</v>
+        <v>55</v>
       </c>
       <c r="E35" t="s">
         <v>9</v>
       </c>
       <c r="F35" t="s">
-        <v>152</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="E36" t="s">
         <v>9</v>
       </c>
       <c r="F36" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>211</v>
-      </c>
-      <c r="C37" t="s">
-        <v>95</v>
+        <v>204</v>
       </c>
       <c r="E37" t="s">
         <v>9</v>
+      </c>
+      <c r="F37" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" t="s">
-        <v>75</v>
+        <v>185</v>
       </c>
       <c r="E38" t="s">
         <v>9</v>
+      </c>
+      <c r="F38" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>134</v>
+        <v>211</v>
       </c>
       <c r="C39" t="s">
         <v>95</v>
@@ -2753,159 +2759,156 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>191</v>
+        <v>12</v>
+      </c>
+      <c r="C40" t="s">
+        <v>75</v>
       </c>
       <c r="E40" t="s">
         <v>9</v>
-      </c>
-      <c r="F40" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>228</v>
+        <v>134</v>
       </c>
       <c r="C41" t="s">
         <v>95</v>
       </c>
       <c r="E41" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>182</v>
-      </c>
-      <c r="C42" t="s">
-        <v>75</v>
+        <v>191</v>
       </c>
       <c r="E42" t="s">
         <v>9</v>
       </c>
       <c r="F42" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>188</v>
+        <v>228</v>
+      </c>
+      <c r="C43" t="s">
+        <v>95</v>
       </c>
       <c r="E43" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" t="s">
-        <v>152</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C44" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E44" t="s">
         <v>9</v>
+      </c>
+      <c r="F44" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>101</v>
-      </c>
-      <c r="C45" t="s">
-        <v>72</v>
+        <v>188</v>
       </c>
       <c r="E45" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="F45" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>205</v>
+        <v>187</v>
+      </c>
+      <c r="C46" t="s">
+        <v>72</v>
       </c>
       <c r="E46" t="s">
         <v>9</v>
-      </c>
-      <c r="F46" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>184</v>
+        <v>101</v>
+      </c>
+      <c r="C47" t="s">
+        <v>72</v>
       </c>
       <c r="E47" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" t="s">
-        <v>72</v>
+        <v>205</v>
       </c>
       <c r="E48" t="s">
         <v>9</v>
+      </c>
+      <c r="F48" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>195</v>
-      </c>
-      <c r="C49" t="s">
-        <v>72</v>
+        <v>184</v>
       </c>
       <c r="E49" t="s">
         <v>9</v>
+      </c>
+      <c r="F49" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>193</v>
+        <v>240</v>
       </c>
       <c r="C50" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="E50" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="C51" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E51" t="s">
         <v>9</v>
-      </c>
-      <c r="F51" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
       <c r="C52" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E52" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>234</v>
+        <v>193</v>
       </c>
       <c r="C53" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="E53" t="s">
         <v>9</v>
@@ -2913,13 +2916,16 @@
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>192</v>
+        <v>76</v>
+      </c>
+      <c r="C54" t="s">
+        <v>75</v>
       </c>
       <c r="E54" t="s">
         <v>9</v>
       </c>
       <c r="F54" t="s">
-        <v>152</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.3">
@@ -2935,32 +2941,40 @@
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>237</v>
+        <v>227</v>
+      </c>
+      <c r="C56" t="s">
+        <v>75</v>
       </c>
       <c r="E56" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" t="s">
-        <v>152</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C57" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="E57" t="s">
         <v>9</v>
       </c>
-      <c r="F57" t="s">
-        <v>239</v>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>192</v>
+      </c>
+      <c r="E58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F54">
-    <sortCondition ref="B54"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F58">
+    <sortCondition ref="B58"/>
   </sortState>
   <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="schlecht">

</xml_diff>